<commit_message>
Enhanced EDP bulk upload functionality with new changes. update on sample data with new header
</commit_message>
<xml_diff>
--- a/public/sample-files/sample_edp_admin.xlsx
+++ b/public/sample-files/sample_edp_admin.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ADMIN\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\OIMS\public\sample-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,19 +26,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>EDP</t>
-  </si>
-  <si>
     <t>Material Description</t>
   </si>
   <si>
     <t>Section</t>
   </si>
   <si>
-    <t>Category</t>
+    <t>UoM</t>
   </si>
   <si>
-    <t>UoM</t>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>Material Group</t>
   </si>
 </sst>
 </file>
@@ -372,8 +372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -382,21 +382,21 @@
     <col min="2" max="2" width="43.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
remove material group from edp sample file
</commit_message>
<xml_diff>
--- a/public/sample-files/sample_edp_admin.xlsx
+++ b/public/sample-files/sample_edp_admin.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Material Description</t>
   </si>
@@ -36,9 +36,6 @@
   </si>
   <si>
     <t>Material</t>
-  </si>
-  <si>
-    <t>Material Group</t>
   </si>
 </sst>
 </file>
@@ -370,10 +367,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -385,7 +382,7 @@
     <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -398,14 +395,11 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
     </row>
   </sheetData>

</xml_diff>